<commit_message>
Correct length to 25ft for tunning C
</commit_message>
<xml_diff>
--- a/DSP/ATA-Backend/Mapping DSP.xlsx
+++ b/DSP/ATA-Backend/Mapping DSP.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4108" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4110" uniqueCount="781">
   <si>
     <t xml:space="preserve">Digitizer</t>
   </si>
@@ -845,7 +845,7 @@
     <t xml:space="preserve">20-B-13Y</t>
   </si>
   <si>
-    <t xml:space="preserve">20-B-14X</t>
+    <t xml:space="preserve">20-C-19Y</t>
   </si>
   <si>
     <t xml:space="preserve">20-B-14Y</t>
@@ -1040,7 +1040,7 @@
     <t xml:space="preserve">C</t>
   </si>
   <si>
-    <t xml:space="preserve">20-C-1X</t>
+    <t xml:space="preserve">25-C-1X</t>
   </si>
   <si>
     <t xml:space="preserve">Att 11</t>
@@ -1052,52 +1052,52 @@
     <t xml:space="preserve">dsp-sw2</t>
   </si>
   <si>
-    <t xml:space="preserve">20-C-1Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-2X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-2Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-3X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-3Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-4X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-4Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-5X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-5Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-6X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-6Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-7X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-7Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-8X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-8Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-9X</t>
+    <t xml:space="preserve">25-C-1Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-2X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-2Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-3X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-3Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-4X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-4Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-5X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-5Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-6X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-6Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-7X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-7Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-8X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-8Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-9X</t>
   </si>
   <si>
     <t xml:space="preserve">Att 12</t>
@@ -1106,52 +1106,52 @@
     <t xml:space="preserve">RFSoC 12</t>
   </si>
   <si>
-    <t xml:space="preserve">20-C-9Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-10X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-10Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-11X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-11Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-12X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-12Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-13X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-13Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-14X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-14Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-15X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-15Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-16X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-16Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-17X</t>
+    <t xml:space="preserve">25-C-9Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-10X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-10Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-11X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-11Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-12X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-12Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-13X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-13Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-14X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-14Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-15X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-15Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-16X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-16Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-17X</t>
   </si>
   <si>
     <t xml:space="preserve">Att 13</t>
@@ -1160,52 +1160,52 @@
     <t xml:space="preserve">RFSoC 13</t>
   </si>
   <si>
-    <t xml:space="preserve">20-C-17Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-18X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-18Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-19X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-19Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-20X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-20Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-21X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-21Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-22X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-22Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-23X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-23Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-24X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-24Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-25X</t>
+    <t xml:space="preserve">25-C-17Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-18X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-18Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-19X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-19Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-20X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-20Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-21X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-21Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-22X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-22Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-23X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-23Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-24X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-24Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-25X</t>
   </si>
   <si>
     <t xml:space="preserve">Att 14</t>
@@ -1214,52 +1214,52 @@
     <t xml:space="preserve">RFSoC 14</t>
   </si>
   <si>
-    <t xml:space="preserve">20-C-25Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-26X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-26Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-27X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-27Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-28X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-28Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-29X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-29Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-30X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-30Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-31X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-31Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-32X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-32Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-33X</t>
+    <t xml:space="preserve">25-C-25Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-26X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-26Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-27X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-27Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-28X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-28Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-29X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-29Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-30X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-30Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-31X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-31Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-32X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-32Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-33X</t>
   </si>
   <si>
     <t xml:space="preserve">Att 15</t>
@@ -1268,61 +1268,61 @@
     <t xml:space="preserve">RFSoC 15</t>
   </si>
   <si>
-    <t xml:space="preserve">20-C-33Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-34X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-34Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-35X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-35Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-36X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-36Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-37X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-37Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-38X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-38Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-39X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-39Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-40X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-40Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-41X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-41Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-42X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-C-42Y</t>
+    <t xml:space="preserve">25-C-33Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-34X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-34Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-35X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-35Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-36X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-36Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-37X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-37Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-38X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-38Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-39X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-39Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-40X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-40Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-41X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-41Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-42X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-C-42Y</t>
   </si>
   <si>
     <t xml:space="preserve">D</t>
@@ -2373,7 +2373,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -2433,6 +2433,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -2687,7 +2693,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="84">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2984,6 +2990,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3095,7 +3113,7 @@
       <selection pane="topLeft" activeCell="P25" activeCellId="0" sqref="P25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3848,11 +3866,11 @@
   </sheetPr>
   <dimension ref="A1:Y347"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K324" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y344" activeCellId="0" sqref="Y344"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F261" activeCellId="0" sqref="F261"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.67"/>
@@ -10530,7 +10548,7 @@
       <c r="E118" s="35" t="n">
         <v>20</v>
       </c>
-      <c r="F118" s="37" t="s">
+      <c r="F118" s="74" t="s">
         <v>274</v>
       </c>
       <c r="G118" s="36"/>
@@ -11639,7 +11657,9 @@
       <c r="C137" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="D137" s="46"/>
+      <c r="D137" s="75" t="s">
+        <v>274</v>
+      </c>
       <c r="E137" s="45" t="n">
         <v>20</v>
       </c>
@@ -12053,8 +12073,8 @@
         <v>243</v>
       </c>
       <c r="D144" s="50"/>
-      <c r="E144" s="49" t="n">
-        <v>20</v>
+      <c r="E144" s="76" t="s">
+        <v>274</v>
       </c>
       <c r="F144" s="51" t="s">
         <v>304</v>
@@ -13936,7 +13956,7 @@
       </c>
       <c r="D178" s="27"/>
       <c r="E178" s="26" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F178" s="27" t="s">
         <v>339</v>
@@ -13999,7 +14019,7 @@
       </c>
       <c r="D179" s="31"/>
       <c r="E179" s="30" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F179" s="31" t="s">
         <v>343</v>
@@ -14058,7 +14078,7 @@
       </c>
       <c r="D180" s="27"/>
       <c r="E180" s="26" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F180" s="27" t="s">
         <v>344</v>
@@ -14115,7 +14135,7 @@
       </c>
       <c r="D181" s="31"/>
       <c r="E181" s="30" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F181" s="31" t="s">
         <v>345</v>
@@ -14174,7 +14194,7 @@
       </c>
       <c r="D182" s="27"/>
       <c r="E182" s="26" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F182" s="27" t="s">
         <v>346</v>
@@ -14231,7 +14251,7 @@
       </c>
       <c r="D183" s="31"/>
       <c r="E183" s="30" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F183" s="31" t="s">
         <v>347</v>
@@ -14290,7 +14310,7 @@
       </c>
       <c r="D184" s="27"/>
       <c r="E184" s="26" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F184" s="27" t="s">
         <v>348</v>
@@ -14347,7 +14367,7 @@
       </c>
       <c r="D185" s="31"/>
       <c r="E185" s="30" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F185" s="31" t="s">
         <v>349</v>
@@ -14406,7 +14426,7 @@
       </c>
       <c r="D186" s="27"/>
       <c r="E186" s="26" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F186" s="27" t="s">
         <v>350</v>
@@ -14469,7 +14489,7 @@
       </c>
       <c r="D187" s="31"/>
       <c r="E187" s="30" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F187" s="31" t="s">
         <v>351</v>
@@ -14528,7 +14548,7 @@
       </c>
       <c r="D188" s="27"/>
       <c r="E188" s="26" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F188" s="27" t="s">
         <v>352</v>
@@ -14585,7 +14605,7 @@
       </c>
       <c r="D189" s="31"/>
       <c r="E189" s="30" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F189" s="31" t="s">
         <v>353</v>
@@ -14644,7 +14664,7 @@
       </c>
       <c r="D190" s="27"/>
       <c r="E190" s="26" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F190" s="27" t="s">
         <v>354</v>
@@ -14701,7 +14721,7 @@
       </c>
       <c r="D191" s="31"/>
       <c r="E191" s="30" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F191" s="31" t="s">
         <v>355</v>
@@ -14760,7 +14780,7 @@
       </c>
       <c r="D192" s="27"/>
       <c r="E192" s="26" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F192" s="32" t="s">
         <v>356</v>
@@ -14817,7 +14837,7 @@
       </c>
       <c r="D193" s="31"/>
       <c r="E193" s="30" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F193" s="33" t="s">
         <v>357</v>
@@ -14876,7 +14896,7 @@
       </c>
       <c r="D194" s="36"/>
       <c r="E194" s="35" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F194" s="37" t="s">
         <v>358</v>
@@ -14939,7 +14959,7 @@
       </c>
       <c r="D195" s="39"/>
       <c r="E195" s="38" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F195" s="40" t="s">
         <v>361</v>
@@ -14998,7 +15018,7 @@
       </c>
       <c r="D196" s="36"/>
       <c r="E196" s="35" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F196" s="37" t="s">
         <v>362</v>
@@ -15055,7 +15075,7 @@
       </c>
       <c r="D197" s="39"/>
       <c r="E197" s="38" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F197" s="40" t="s">
         <v>363</v>
@@ -15114,7 +15134,7 @@
       </c>
       <c r="D198" s="36"/>
       <c r="E198" s="35" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F198" s="37" t="s">
         <v>364</v>
@@ -15171,7 +15191,7 @@
       </c>
       <c r="D199" s="39"/>
       <c r="E199" s="38" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F199" s="40" t="s">
         <v>365</v>
@@ -15230,7 +15250,7 @@
       </c>
       <c r="D200" s="36"/>
       <c r="E200" s="35" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F200" s="37" t="s">
         <v>366</v>
@@ -15287,7 +15307,7 @@
       </c>
       <c r="D201" s="39"/>
       <c r="E201" s="38" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F201" s="40" t="s">
         <v>367</v>
@@ -15346,7 +15366,7 @@
       </c>
       <c r="D202" s="36"/>
       <c r="E202" s="35" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F202" s="37" t="s">
         <v>368</v>
@@ -15409,7 +15429,7 @@
       </c>
       <c r="D203" s="39"/>
       <c r="E203" s="38" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F203" s="40" t="s">
         <v>369</v>
@@ -15468,7 +15488,7 @@
       </c>
       <c r="D204" s="36"/>
       <c r="E204" s="35" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F204" s="37" t="s">
         <v>370</v>
@@ -15525,7 +15545,7 @@
       </c>
       <c r="D205" s="39"/>
       <c r="E205" s="38" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F205" s="40" t="s">
         <v>371</v>
@@ -15584,7 +15604,7 @@
       </c>
       <c r="D206" s="36"/>
       <c r="E206" s="35" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F206" s="37" t="s">
         <v>372</v>
@@ -15641,7 +15661,7 @@
       </c>
       <c r="D207" s="39"/>
       <c r="E207" s="38" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F207" s="40" t="s">
         <v>373</v>
@@ -15700,7 +15720,7 @@
       </c>
       <c r="D208" s="36"/>
       <c r="E208" s="35" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F208" s="37" t="s">
         <v>374</v>
@@ -15757,7 +15777,7 @@
       </c>
       <c r="D209" s="39"/>
       <c r="E209" s="38" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F209" s="40" t="s">
         <v>375</v>
@@ -15816,7 +15836,7 @@
       </c>
       <c r="D210" s="43"/>
       <c r="E210" s="42" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F210" s="44" t="s">
         <v>376</v>
@@ -15879,7 +15899,7 @@
       </c>
       <c r="D211" s="46"/>
       <c r="E211" s="45" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F211" s="47" t="s">
         <v>379</v>
@@ -15938,7 +15958,7 @@
       </c>
       <c r="D212" s="43"/>
       <c r="E212" s="42" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F212" s="44" t="s">
         <v>380</v>
@@ -15995,7 +16015,7 @@
       </c>
       <c r="D213" s="46"/>
       <c r="E213" s="45" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F213" s="47" t="s">
         <v>381</v>
@@ -16054,7 +16074,7 @@
       </c>
       <c r="D214" s="43"/>
       <c r="E214" s="42" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F214" s="44" t="s">
         <v>382</v>
@@ -16111,7 +16131,7 @@
       </c>
       <c r="D215" s="46"/>
       <c r="E215" s="45" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F215" s="47" t="s">
         <v>383</v>
@@ -16170,7 +16190,7 @@
       </c>
       <c r="D216" s="43"/>
       <c r="E216" s="42" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F216" s="44" t="s">
         <v>384</v>
@@ -16227,7 +16247,7 @@
       </c>
       <c r="D217" s="46"/>
       <c r="E217" s="45" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F217" s="47" t="s">
         <v>385</v>
@@ -16286,7 +16306,7 @@
       </c>
       <c r="D218" s="43"/>
       <c r="E218" s="42" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F218" s="44" t="s">
         <v>386</v>
@@ -16349,7 +16369,7 @@
       </c>
       <c r="D219" s="46"/>
       <c r="E219" s="45" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F219" s="47" t="s">
         <v>387</v>
@@ -16408,7 +16428,7 @@
       </c>
       <c r="D220" s="43"/>
       <c r="E220" s="42" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F220" s="44" t="s">
         <v>388</v>
@@ -16465,7 +16485,7 @@
       </c>
       <c r="D221" s="46"/>
       <c r="E221" s="45" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F221" s="47" t="s">
         <v>389</v>
@@ -16524,7 +16544,7 @@
       </c>
       <c r="D222" s="43"/>
       <c r="E222" s="42" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F222" s="44" t="s">
         <v>390</v>
@@ -16581,7 +16601,7 @@
       </c>
       <c r="D223" s="46"/>
       <c r="E223" s="45" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F223" s="47" t="s">
         <v>391</v>
@@ -16640,7 +16660,7 @@
       </c>
       <c r="D224" s="43"/>
       <c r="E224" s="42" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F224" s="44" t="s">
         <v>392</v>
@@ -16697,7 +16717,7 @@
       </c>
       <c r="D225" s="46"/>
       <c r="E225" s="45" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F225" s="47" t="s">
         <v>393</v>
@@ -16756,7 +16776,7 @@
       </c>
       <c r="D226" s="50"/>
       <c r="E226" s="49" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F226" s="51" t="s">
         <v>394</v>
@@ -16819,7 +16839,7 @@
       </c>
       <c r="D227" s="53"/>
       <c r="E227" s="52" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F227" s="54" t="s">
         <v>397</v>
@@ -16878,7 +16898,7 @@
       </c>
       <c r="D228" s="50"/>
       <c r="E228" s="49" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F228" s="51" t="s">
         <v>398</v>
@@ -16935,7 +16955,7 @@
       </c>
       <c r="D229" s="53"/>
       <c r="E229" s="52" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F229" s="54" t="s">
         <v>399</v>
@@ -16994,7 +17014,7 @@
       </c>
       <c r="D230" s="50"/>
       <c r="E230" s="49" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F230" s="51" t="s">
         <v>400</v>
@@ -17051,7 +17071,7 @@
       </c>
       <c r="D231" s="53"/>
       <c r="E231" s="52" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F231" s="54" t="s">
         <v>401</v>
@@ -17110,7 +17130,7 @@
       </c>
       <c r="D232" s="50"/>
       <c r="E232" s="49" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F232" s="51" t="s">
         <v>402</v>
@@ -17167,7 +17187,7 @@
       </c>
       <c r="D233" s="53"/>
       <c r="E233" s="52" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F233" s="54" t="s">
         <v>403</v>
@@ -17226,7 +17246,7 @@
       </c>
       <c r="D234" s="50"/>
       <c r="E234" s="49" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F234" s="51" t="s">
         <v>404</v>
@@ -17289,7 +17309,7 @@
       </c>
       <c r="D235" s="53"/>
       <c r="E235" s="52" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F235" s="54" t="s">
         <v>405</v>
@@ -17348,7 +17368,7 @@
       </c>
       <c r="D236" s="50"/>
       <c r="E236" s="49" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F236" s="51" t="s">
         <v>406</v>
@@ -17405,7 +17425,7 @@
       </c>
       <c r="D237" s="53"/>
       <c r="E237" s="52" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F237" s="54" t="s">
         <v>407</v>
@@ -17464,7 +17484,7 @@
       </c>
       <c r="D238" s="50"/>
       <c r="E238" s="49" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F238" s="51" t="s">
         <v>408</v>
@@ -17521,7 +17541,7 @@
       </c>
       <c r="D239" s="53"/>
       <c r="E239" s="52" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F239" s="54" t="s">
         <v>409</v>
@@ -17580,7 +17600,7 @@
       </c>
       <c r="D240" s="50"/>
       <c r="E240" s="49" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F240" s="51" t="s">
         <v>410</v>
@@ -17637,7 +17657,7 @@
       </c>
       <c r="D241" s="53"/>
       <c r="E241" s="52" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F241" s="54" t="s">
         <v>411</v>
@@ -17696,7 +17716,7 @@
       </c>
       <c r="D242" s="57"/>
       <c r="E242" s="56" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F242" s="58" t="s">
         <v>412</v>
@@ -17759,7 +17779,7 @@
       </c>
       <c r="D243" s="60"/>
       <c r="E243" s="59" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F243" s="61" t="s">
         <v>415</v>
@@ -17818,7 +17838,7 @@
       </c>
       <c r="D244" s="57"/>
       <c r="E244" s="56" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F244" s="58" t="s">
         <v>416</v>
@@ -17875,7 +17895,7 @@
       </c>
       <c r="D245" s="60"/>
       <c r="E245" s="59" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F245" s="61" t="s">
         <v>417</v>
@@ -17934,7 +17954,7 @@
       </c>
       <c r="D246" s="57"/>
       <c r="E246" s="56" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F246" s="58" t="s">
         <v>418</v>
@@ -17991,7 +18011,7 @@
       </c>
       <c r="D247" s="60"/>
       <c r="E247" s="59" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F247" s="61" t="s">
         <v>419</v>
@@ -18050,7 +18070,7 @@
       </c>
       <c r="D248" s="57"/>
       <c r="E248" s="56" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F248" s="58" t="s">
         <v>420</v>
@@ -18107,7 +18127,7 @@
       </c>
       <c r="D249" s="60"/>
       <c r="E249" s="59" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F249" s="61" t="s">
         <v>421</v>
@@ -18166,7 +18186,7 @@
       </c>
       <c r="D250" s="57"/>
       <c r="E250" s="56" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F250" s="58" t="s">
         <v>422</v>
@@ -18229,7 +18249,7 @@
       </c>
       <c r="D251" s="60"/>
       <c r="E251" s="59" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F251" s="61" t="s">
         <v>423</v>
@@ -18288,7 +18308,7 @@
       </c>
       <c r="D252" s="57"/>
       <c r="E252" s="56" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F252" s="58" t="s">
         <v>424</v>
@@ -18345,7 +18365,7 @@
       </c>
       <c r="D253" s="60"/>
       <c r="E253" s="59" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F253" s="61" t="s">
         <v>425</v>
@@ -18404,7 +18424,7 @@
       </c>
       <c r="D254" s="57"/>
       <c r="E254" s="56" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F254" s="58" t="s">
         <v>426</v>
@@ -18461,7 +18481,7 @@
       </c>
       <c r="D255" s="60"/>
       <c r="E255" s="59" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F255" s="61" t="s">
         <v>427</v>
@@ -18520,7 +18540,7 @@
       </c>
       <c r="D256" s="57"/>
       <c r="E256" s="56" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F256" s="58" t="s">
         <v>428</v>
@@ -18577,7 +18597,7 @@
       </c>
       <c r="D257" s="60"/>
       <c r="E257" s="59" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F257" s="61" t="s">
         <v>429</v>
@@ -18636,7 +18656,7 @@
       </c>
       <c r="D258" s="64"/>
       <c r="E258" s="63" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F258" s="65" t="s">
         <v>430</v>
@@ -18699,7 +18719,7 @@
       </c>
       <c r="D259" s="67"/>
       <c r="E259" s="66" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F259" s="68" t="s">
         <v>431</v>
@@ -18758,7 +18778,7 @@
       </c>
       <c r="D260" s="64"/>
       <c r="E260" s="63" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F260" s="65" t="s">
         <v>432</v>
@@ -18815,7 +18835,7 @@
       </c>
       <c r="D261" s="67"/>
       <c r="E261" s="66" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F261" s="68" t="s">
         <v>433</v>
@@ -20745,58 +20765,58 @@
       <c r="Y295" s="29"/>
     </row>
     <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A296" s="74" t="s">
+      <c r="A296" s="77" t="s">
         <v>157</v>
       </c>
-      <c r="B296" s="75" t="s">
+      <c r="B296" s="78" t="s">
         <v>97</v>
       </c>
-      <c r="C296" s="75" t="s">
+      <c r="C296" s="78" t="s">
         <v>434</v>
       </c>
-      <c r="D296" s="76"/>
-      <c r="E296" s="75" t="n">
-        <v>20</v>
-      </c>
-      <c r="F296" s="77" t="s">
+      <c r="D296" s="79"/>
+      <c r="E296" s="78" t="n">
+        <v>20</v>
+      </c>
+      <c r="F296" s="80" t="s">
         <v>567</v>
       </c>
-      <c r="G296" s="76"/>
-      <c r="H296" s="75" t="s">
+      <c r="G296" s="79"/>
+      <c r="H296" s="78" t="s">
         <v>568</v>
       </c>
-      <c r="I296" s="75" t="s">
+      <c r="I296" s="78" t="s">
         <v>569</v>
       </c>
-      <c r="J296" s="76"/>
-      <c r="K296" s="75" t="n">
+      <c r="J296" s="79"/>
+      <c r="K296" s="78" t="n">
         <v>25</v>
       </c>
-      <c r="L296" s="77" t="s">
+      <c r="L296" s="80" t="s">
         <v>570</v>
       </c>
-      <c r="M296" s="76"/>
-      <c r="N296" s="75" t="n">
+      <c r="M296" s="79"/>
+      <c r="N296" s="78" t="n">
         <v>1</v>
       </c>
-      <c r="O296" s="76" t="s">
+      <c r="O296" s="79" t="s">
         <v>571</v>
       </c>
-      <c r="P296" s="75" t="n">
+      <c r="P296" s="78" t="n">
         <v>1</v>
       </c>
-      <c r="Q296" s="76"/>
-      <c r="R296" s="76" t="s">
-        <v>102</v>
-      </c>
-      <c r="S296" s="76" t="s">
-        <v>103</v>
-      </c>
-      <c r="T296" s="76"/>
-      <c r="U296" s="75" t="n">
+      <c r="Q296" s="79"/>
+      <c r="R296" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="S296" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="T296" s="79"/>
+      <c r="U296" s="78" t="n">
         <v>1</v>
       </c>
-      <c r="V296" s="76" t="s">
+      <c r="V296" s="79" t="s">
         <v>572</v>
       </c>
       <c r="W296" s="28" t="s">
@@ -20810,56 +20830,56 @@
       </c>
     </row>
     <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A297" s="74"/>
-      <c r="B297" s="78" t="s">
+      <c r="A297" s="77"/>
+      <c r="B297" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="C297" s="78" t="s">
+      <c r="C297" s="81" t="s">
         <v>434</v>
       </c>
-      <c r="D297" s="79"/>
-      <c r="E297" s="78" t="n">
-        <v>20</v>
-      </c>
-      <c r="F297" s="80" t="s">
+      <c r="D297" s="82"/>
+      <c r="E297" s="81" t="n">
+        <v>20</v>
+      </c>
+      <c r="F297" s="83" t="s">
         <v>573</v>
       </c>
-      <c r="G297" s="79"/>
-      <c r="H297" s="78" t="s">
+      <c r="G297" s="82"/>
+      <c r="H297" s="81" t="s">
         <v>574</v>
       </c>
-      <c r="I297" s="78" t="s">
+      <c r="I297" s="81" t="s">
         <v>575</v>
       </c>
-      <c r="J297" s="79"/>
-      <c r="K297" s="78" t="n">
+      <c r="J297" s="82"/>
+      <c r="K297" s="81" t="n">
         <v>25</v>
       </c>
-      <c r="L297" s="80" t="s">
+      <c r="L297" s="83" t="s">
         <v>576</v>
       </c>
-      <c r="M297" s="79"/>
-      <c r="N297" s="78" t="n">
+      <c r="M297" s="82"/>
+      <c r="N297" s="81" t="n">
         <v>2</v>
       </c>
-      <c r="O297" s="79" t="s">
+      <c r="O297" s="82" t="s">
         <v>571</v>
       </c>
-      <c r="P297" s="78" t="n">
+      <c r="P297" s="81" t="n">
         <v>2</v>
       </c>
-      <c r="Q297" s="79"/>
-      <c r="R297" s="79" t="s">
-        <v>102</v>
-      </c>
-      <c r="S297" s="79" t="s">
-        <v>103</v>
-      </c>
-      <c r="T297" s="79"/>
-      <c r="U297" s="78" t="n">
+      <c r="Q297" s="82"/>
+      <c r="R297" s="82" t="s">
+        <v>102</v>
+      </c>
+      <c r="S297" s="82" t="s">
+        <v>103</v>
+      </c>
+      <c r="T297" s="82"/>
+      <c r="U297" s="81" t="n">
         <v>2</v>
       </c>
-      <c r="V297" s="79" t="s">
+      <c r="V297" s="82" t="s">
         <v>572</v>
       </c>
       <c r="W297" s="28"/>
@@ -20867,58 +20887,58 @@
       <c r="Y297" s="29"/>
     </row>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A298" s="74" t="s">
+      <c r="A298" s="77" t="s">
         <v>162</v>
       </c>
-      <c r="B298" s="75" t="s">
+      <c r="B298" s="78" t="s">
         <v>97</v>
       </c>
-      <c r="C298" s="75" t="s">
+      <c r="C298" s="78" t="s">
         <v>434</v>
       </c>
-      <c r="D298" s="76"/>
-      <c r="E298" s="75" t="n">
-        <v>20</v>
-      </c>
-      <c r="F298" s="77" t="s">
+      <c r="D298" s="79"/>
+      <c r="E298" s="78" t="n">
+        <v>20</v>
+      </c>
+      <c r="F298" s="80" t="s">
         <v>577</v>
       </c>
-      <c r="G298" s="76"/>
-      <c r="H298" s="75" t="s">
+      <c r="G298" s="79"/>
+      <c r="H298" s="78" t="s">
         <v>578</v>
       </c>
-      <c r="I298" s="75" t="s">
+      <c r="I298" s="78" t="s">
         <v>579</v>
       </c>
-      <c r="J298" s="76"/>
-      <c r="K298" s="75" t="n">
+      <c r="J298" s="79"/>
+      <c r="K298" s="78" t="n">
         <v>25</v>
       </c>
-      <c r="L298" s="77" t="s">
+      <c r="L298" s="80" t="s">
         <v>580</v>
       </c>
-      <c r="M298" s="76"/>
-      <c r="N298" s="75" t="n">
+      <c r="M298" s="79"/>
+      <c r="N298" s="78" t="n">
         <v>3</v>
       </c>
-      <c r="O298" s="76" t="s">
+      <c r="O298" s="79" t="s">
         <v>571</v>
       </c>
-      <c r="P298" s="75" t="n">
+      <c r="P298" s="78" t="n">
         <v>3</v>
       </c>
-      <c r="Q298" s="76"/>
-      <c r="R298" s="76" t="s">
-        <v>102</v>
-      </c>
-      <c r="S298" s="76" t="s">
-        <v>103</v>
-      </c>
-      <c r="T298" s="76"/>
-      <c r="U298" s="75" t="n">
+      <c r="Q298" s="79"/>
+      <c r="R298" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="S298" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="T298" s="79"/>
+      <c r="U298" s="78" t="n">
         <v>3</v>
       </c>
-      <c r="V298" s="76" t="s">
+      <c r="V298" s="79" t="s">
         <v>572</v>
       </c>
       <c r="W298" s="28"/>
@@ -20926,56 +20946,56 @@
       <c r="Y298" s="29"/>
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A299" s="74"/>
-      <c r="B299" s="78" t="s">
+      <c r="A299" s="77"/>
+      <c r="B299" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="C299" s="78" t="s">
+      <c r="C299" s="81" t="s">
         <v>434</v>
       </c>
-      <c r="D299" s="79"/>
-      <c r="E299" s="78" t="n">
-        <v>20</v>
-      </c>
-      <c r="F299" s="80" t="s">
+      <c r="D299" s="82"/>
+      <c r="E299" s="81" t="n">
+        <v>20</v>
+      </c>
+      <c r="F299" s="83" t="s">
         <v>581</v>
       </c>
-      <c r="G299" s="79"/>
-      <c r="H299" s="78" t="s">
+      <c r="G299" s="82"/>
+      <c r="H299" s="81" t="s">
         <v>582</v>
       </c>
-      <c r="I299" s="78" t="s">
+      <c r="I299" s="81" t="s">
         <v>583</v>
       </c>
-      <c r="J299" s="79"/>
-      <c r="K299" s="78" t="n">
+      <c r="J299" s="82"/>
+      <c r="K299" s="81" t="n">
         <v>25</v>
       </c>
-      <c r="L299" s="80" t="s">
+      <c r="L299" s="83" t="s">
         <v>584</v>
       </c>
-      <c r="M299" s="79"/>
-      <c r="N299" s="78" t="n">
+      <c r="M299" s="82"/>
+      <c r="N299" s="81" t="n">
         <v>4</v>
       </c>
-      <c r="O299" s="79" t="s">
+      <c r="O299" s="82" t="s">
         <v>571</v>
       </c>
-      <c r="P299" s="78" t="n">
+      <c r="P299" s="81" t="n">
         <v>4</v>
       </c>
-      <c r="Q299" s="79"/>
-      <c r="R299" s="79" t="s">
-        <v>102</v>
-      </c>
-      <c r="S299" s="79" t="s">
-        <v>103</v>
-      </c>
-      <c r="T299" s="79"/>
-      <c r="U299" s="78" t="n">
+      <c r="Q299" s="82"/>
+      <c r="R299" s="82" t="s">
+        <v>102</v>
+      </c>
+      <c r="S299" s="82" t="s">
+        <v>103</v>
+      </c>
+      <c r="T299" s="82"/>
+      <c r="U299" s="81" t="n">
         <v>4</v>
       </c>
-      <c r="V299" s="79" t="s">
+      <c r="V299" s="82" t="s">
         <v>572</v>
       </c>
       <c r="W299" s="28"/>
@@ -20983,58 +21003,58 @@
       <c r="Y299" s="29"/>
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A300" s="74" t="s">
+      <c r="A300" s="77" t="s">
         <v>165</v>
       </c>
-      <c r="B300" s="75" t="s">
+      <c r="B300" s="78" t="s">
         <v>97</v>
       </c>
-      <c r="C300" s="75" t="s">
+      <c r="C300" s="78" t="s">
         <v>434</v>
       </c>
-      <c r="D300" s="76"/>
-      <c r="E300" s="75" t="n">
-        <v>20</v>
-      </c>
-      <c r="F300" s="77" t="s">
+      <c r="D300" s="79"/>
+      <c r="E300" s="78" t="n">
+        <v>20</v>
+      </c>
+      <c r="F300" s="80" t="s">
         <v>585</v>
       </c>
-      <c r="G300" s="76"/>
-      <c r="H300" s="75" t="s">
+      <c r="G300" s="79"/>
+      <c r="H300" s="78" t="s">
         <v>586</v>
       </c>
-      <c r="I300" s="75" t="s">
+      <c r="I300" s="78" t="s">
         <v>587</v>
       </c>
-      <c r="J300" s="76"/>
-      <c r="K300" s="75" t="n">
+      <c r="J300" s="79"/>
+      <c r="K300" s="78" t="n">
         <v>25</v>
       </c>
-      <c r="L300" s="77" t="s">
+      <c r="L300" s="80" t="s">
         <v>588</v>
       </c>
-      <c r="M300" s="76"/>
-      <c r="N300" s="75" t="n">
+      <c r="M300" s="79"/>
+      <c r="N300" s="78" t="n">
         <v>5</v>
       </c>
-      <c r="O300" s="76" t="s">
+      <c r="O300" s="79" t="s">
         <v>571</v>
       </c>
-      <c r="P300" s="75" t="n">
+      <c r="P300" s="78" t="n">
         <v>5</v>
       </c>
-      <c r="Q300" s="76"/>
-      <c r="R300" s="76" t="s">
-        <v>102</v>
-      </c>
-      <c r="S300" s="76" t="s">
-        <v>103</v>
-      </c>
-      <c r="T300" s="76"/>
-      <c r="U300" s="75" t="n">
+      <c r="Q300" s="79"/>
+      <c r="R300" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="S300" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="T300" s="79"/>
+      <c r="U300" s="78" t="n">
         <v>5</v>
       </c>
-      <c r="V300" s="76" t="s">
+      <c r="V300" s="79" t="s">
         <v>572</v>
       </c>
       <c r="W300" s="28"/>
@@ -21042,56 +21062,56 @@
       <c r="Y300" s="29"/>
     </row>
     <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A301" s="74"/>
-      <c r="B301" s="78" t="s">
+      <c r="A301" s="77"/>
+      <c r="B301" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="C301" s="78" t="s">
+      <c r="C301" s="81" t="s">
         <v>434</v>
       </c>
-      <c r="D301" s="79"/>
-      <c r="E301" s="78" t="n">
-        <v>20</v>
-      </c>
-      <c r="F301" s="80" t="s">
+      <c r="D301" s="82"/>
+      <c r="E301" s="81" t="n">
+        <v>20</v>
+      </c>
+      <c r="F301" s="83" t="s">
         <v>589</v>
       </c>
-      <c r="G301" s="79"/>
-      <c r="H301" s="78" t="s">
+      <c r="G301" s="82"/>
+      <c r="H301" s="81" t="s">
         <v>590</v>
       </c>
-      <c r="I301" s="78" t="s">
+      <c r="I301" s="81" t="s">
         <v>591</v>
       </c>
-      <c r="J301" s="79"/>
-      <c r="K301" s="78" t="n">
+      <c r="J301" s="82"/>
+      <c r="K301" s="81" t="n">
         <v>25</v>
       </c>
-      <c r="L301" s="80" t="s">
+      <c r="L301" s="83" t="s">
         <v>592</v>
       </c>
-      <c r="M301" s="79"/>
-      <c r="N301" s="78" t="n">
+      <c r="M301" s="82"/>
+      <c r="N301" s="81" t="n">
         <v>6</v>
       </c>
-      <c r="O301" s="79" t="s">
+      <c r="O301" s="82" t="s">
         <v>571</v>
       </c>
-      <c r="P301" s="78" t="n">
+      <c r="P301" s="81" t="n">
         <v>6</v>
       </c>
-      <c r="Q301" s="79"/>
-      <c r="R301" s="79" t="s">
-        <v>102</v>
-      </c>
-      <c r="S301" s="79" t="s">
-        <v>103</v>
-      </c>
-      <c r="T301" s="79"/>
-      <c r="U301" s="78" t="n">
+      <c r="Q301" s="82"/>
+      <c r="R301" s="82" t="s">
+        <v>102</v>
+      </c>
+      <c r="S301" s="82" t="s">
+        <v>103</v>
+      </c>
+      <c r="T301" s="82"/>
+      <c r="U301" s="81" t="n">
         <v>6</v>
       </c>
-      <c r="V301" s="79" t="s">
+      <c r="V301" s="82" t="s">
         <v>572</v>
       </c>
       <c r="W301" s="28"/>
@@ -21099,58 +21119,58 @@
       <c r="Y301" s="29"/>
     </row>
     <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A302" s="74" t="s">
+      <c r="A302" s="77" t="s">
         <v>168</v>
       </c>
-      <c r="B302" s="75" t="s">
+      <c r="B302" s="78" t="s">
         <v>97</v>
       </c>
-      <c r="C302" s="75" t="s">
+      <c r="C302" s="78" t="s">
         <v>434</v>
       </c>
-      <c r="D302" s="76"/>
-      <c r="E302" s="75" t="n">
-        <v>20</v>
-      </c>
-      <c r="F302" s="77" t="s">
+      <c r="D302" s="79"/>
+      <c r="E302" s="78" t="n">
+        <v>20</v>
+      </c>
+      <c r="F302" s="80" t="s">
         <v>593</v>
       </c>
-      <c r="G302" s="76"/>
-      <c r="H302" s="75" t="s">
+      <c r="G302" s="79"/>
+      <c r="H302" s="78" t="s">
         <v>594</v>
       </c>
-      <c r="I302" s="75" t="s">
+      <c r="I302" s="78" t="s">
         <v>595</v>
       </c>
-      <c r="J302" s="76"/>
-      <c r="K302" s="75" t="n">
+      <c r="J302" s="79"/>
+      <c r="K302" s="78" t="n">
         <v>25</v>
       </c>
-      <c r="L302" s="77" t="s">
+      <c r="L302" s="80" t="s">
         <v>596</v>
       </c>
-      <c r="M302" s="76"/>
-      <c r="N302" s="75" t="n">
+      <c r="M302" s="79"/>
+      <c r="N302" s="78" t="n">
         <v>7</v>
       </c>
-      <c r="O302" s="76" t="s">
+      <c r="O302" s="79" t="s">
         <v>571</v>
       </c>
-      <c r="P302" s="75" t="n">
+      <c r="P302" s="78" t="n">
         <v>7</v>
       </c>
-      <c r="Q302" s="76"/>
-      <c r="R302" s="76" t="s">
-        <v>102</v>
-      </c>
-      <c r="S302" s="76" t="s">
-        <v>103</v>
-      </c>
-      <c r="T302" s="76"/>
-      <c r="U302" s="75" t="n">
+      <c r="Q302" s="79"/>
+      <c r="R302" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="S302" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="T302" s="79"/>
+      <c r="U302" s="78" t="n">
         <v>7</v>
       </c>
-      <c r="V302" s="76" t="s">
+      <c r="V302" s="79" t="s">
         <v>572</v>
       </c>
       <c r="W302" s="28"/>
@@ -21158,56 +21178,56 @@
       <c r="Y302" s="29"/>
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A303" s="74"/>
-      <c r="B303" s="78" t="s">
+      <c r="A303" s="77"/>
+      <c r="B303" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="C303" s="78" t="s">
+      <c r="C303" s="81" t="s">
         <v>434</v>
       </c>
-      <c r="D303" s="79"/>
-      <c r="E303" s="78" t="n">
-        <v>20</v>
-      </c>
-      <c r="F303" s="80" t="s">
+      <c r="D303" s="82"/>
+      <c r="E303" s="81" t="n">
+        <v>20</v>
+      </c>
+      <c r="F303" s="83" t="s">
         <v>597</v>
       </c>
-      <c r="G303" s="79"/>
-      <c r="H303" s="78" t="s">
+      <c r="G303" s="82"/>
+      <c r="H303" s="81" t="s">
         <v>598</v>
       </c>
-      <c r="I303" s="78" t="s">
+      <c r="I303" s="81" t="s">
         <v>599</v>
       </c>
-      <c r="J303" s="79"/>
-      <c r="K303" s="78" t="n">
+      <c r="J303" s="82"/>
+      <c r="K303" s="81" t="n">
         <v>25</v>
       </c>
-      <c r="L303" s="80" t="s">
+      <c r="L303" s="83" t="s">
         <v>600</v>
       </c>
-      <c r="M303" s="79"/>
-      <c r="N303" s="78" t="n">
+      <c r="M303" s="82"/>
+      <c r="N303" s="81" t="n">
         <v>8</v>
       </c>
-      <c r="O303" s="79" t="s">
+      <c r="O303" s="82" t="s">
         <v>571</v>
       </c>
-      <c r="P303" s="78" t="n">
+      <c r="P303" s="81" t="n">
         <v>8</v>
       </c>
-      <c r="Q303" s="79"/>
-      <c r="R303" s="79" t="s">
-        <v>102</v>
-      </c>
-      <c r="S303" s="79" t="s">
-        <v>103</v>
-      </c>
-      <c r="T303" s="79"/>
-      <c r="U303" s="78" t="n">
+      <c r="Q303" s="82"/>
+      <c r="R303" s="82" t="s">
+        <v>102</v>
+      </c>
+      <c r="S303" s="82" t="s">
+        <v>103</v>
+      </c>
+      <c r="T303" s="82"/>
+      <c r="U303" s="81" t="n">
         <v>8</v>
       </c>
-      <c r="V303" s="79" t="s">
+      <c r="V303" s="82" t="s">
         <v>572</v>
       </c>
       <c r="W303" s="28"/>
@@ -21215,58 +21235,58 @@
       <c r="Y303" s="29"/>
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A304" s="74" t="s">
+      <c r="A304" s="77" t="s">
         <v>171</v>
       </c>
-      <c r="B304" s="75" t="s">
+      <c r="B304" s="78" t="s">
         <v>97</v>
       </c>
-      <c r="C304" s="75" t="s">
+      <c r="C304" s="78" t="s">
         <v>434</v>
       </c>
-      <c r="D304" s="76"/>
-      <c r="E304" s="75" t="n">
-        <v>20</v>
-      </c>
-      <c r="F304" s="77" t="s">
+      <c r="D304" s="79"/>
+      <c r="E304" s="78" t="n">
+        <v>20</v>
+      </c>
+      <c r="F304" s="80" t="s">
         <v>601</v>
       </c>
-      <c r="G304" s="76"/>
-      <c r="H304" s="75" t="s">
+      <c r="G304" s="79"/>
+      <c r="H304" s="78" t="s">
         <v>602</v>
       </c>
-      <c r="I304" s="75" t="s">
+      <c r="I304" s="78" t="s">
         <v>603</v>
       </c>
-      <c r="J304" s="76"/>
-      <c r="K304" s="75" t="n">
+      <c r="J304" s="79"/>
+      <c r="K304" s="78" t="n">
         <v>25</v>
       </c>
-      <c r="L304" s="77" t="s">
+      <c r="L304" s="80" t="s">
         <v>604</v>
       </c>
-      <c r="M304" s="76"/>
-      <c r="N304" s="75" t="n">
+      <c r="M304" s="79"/>
+      <c r="N304" s="78" t="n">
         <v>9</v>
       </c>
-      <c r="O304" s="76" t="s">
+      <c r="O304" s="79" t="s">
         <v>571</v>
       </c>
-      <c r="P304" s="75" t="n">
+      <c r="P304" s="78" t="n">
         <v>9</v>
       </c>
-      <c r="Q304" s="76"/>
-      <c r="R304" s="76" t="s">
-        <v>102</v>
-      </c>
-      <c r="S304" s="76" t="s">
-        <v>103</v>
-      </c>
-      <c r="T304" s="76"/>
-      <c r="U304" s="75" t="n">
+      <c r="Q304" s="79"/>
+      <c r="R304" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="S304" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="T304" s="79"/>
+      <c r="U304" s="78" t="n">
         <v>9</v>
       </c>
-      <c r="V304" s="76" t="s">
+      <c r="V304" s="79" t="s">
         <v>572</v>
       </c>
       <c r="W304" s="28" t="s">
@@ -21280,56 +21300,56 @@
       </c>
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A305" s="74"/>
-      <c r="B305" s="78" t="s">
+      <c r="A305" s="77"/>
+      <c r="B305" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="C305" s="78" t="s">
+      <c r="C305" s="81" t="s">
         <v>434</v>
       </c>
-      <c r="D305" s="79"/>
-      <c r="E305" s="78" t="n">
-        <v>20</v>
-      </c>
-      <c r="F305" s="80" t="s">
+      <c r="D305" s="82"/>
+      <c r="E305" s="81" t="n">
+        <v>20</v>
+      </c>
+      <c r="F305" s="83" t="s">
         <v>605</v>
       </c>
-      <c r="G305" s="79"/>
-      <c r="H305" s="78" t="s">
+      <c r="G305" s="82"/>
+      <c r="H305" s="81" t="s">
         <v>606</v>
       </c>
-      <c r="I305" s="78" t="s">
+      <c r="I305" s="81" t="s">
         <v>607</v>
       </c>
-      <c r="J305" s="79"/>
-      <c r="K305" s="78" t="n">
+      <c r="J305" s="82"/>
+      <c r="K305" s="81" t="n">
         <v>25</v>
       </c>
-      <c r="L305" s="80" t="s">
+      <c r="L305" s="83" t="s">
         <v>608</v>
       </c>
-      <c r="M305" s="79"/>
-      <c r="N305" s="78" t="n">
+      <c r="M305" s="82"/>
+      <c r="N305" s="81" t="n">
         <v>10</v>
       </c>
-      <c r="O305" s="79" t="s">
+      <c r="O305" s="82" t="s">
         <v>571</v>
       </c>
-      <c r="P305" s="78" t="n">
+      <c r="P305" s="81" t="n">
         <v>10</v>
       </c>
-      <c r="Q305" s="79"/>
-      <c r="R305" s="79" t="s">
-        <v>102</v>
-      </c>
-      <c r="S305" s="79" t="s">
-        <v>103</v>
-      </c>
-      <c r="T305" s="79"/>
-      <c r="U305" s="78" t="n">
+      <c r="Q305" s="82"/>
+      <c r="R305" s="82" t="s">
+        <v>102</v>
+      </c>
+      <c r="S305" s="82" t="s">
+        <v>103</v>
+      </c>
+      <c r="T305" s="82"/>
+      <c r="U305" s="81" t="n">
         <v>10</v>
       </c>
-      <c r="V305" s="79" t="s">
+      <c r="V305" s="82" t="s">
         <v>572</v>
       </c>
       <c r="W305" s="28"/>
@@ -21337,58 +21357,58 @@
       <c r="Y305" s="29"/>
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A306" s="74" t="s">
+      <c r="A306" s="77" t="s">
         <v>174</v>
       </c>
-      <c r="B306" s="75" t="s">
+      <c r="B306" s="78" t="s">
         <v>97</v>
       </c>
-      <c r="C306" s="75" t="s">
+      <c r="C306" s="78" t="s">
         <v>434</v>
       </c>
-      <c r="D306" s="76"/>
-      <c r="E306" s="75" t="n">
-        <v>20</v>
-      </c>
-      <c r="F306" s="77" t="s">
+      <c r="D306" s="79"/>
+      <c r="E306" s="78" t="n">
+        <v>20</v>
+      </c>
+      <c r="F306" s="80" t="s">
         <v>609</v>
       </c>
-      <c r="G306" s="76"/>
-      <c r="H306" s="75" t="s">
+      <c r="G306" s="79"/>
+      <c r="H306" s="78" t="s">
         <v>610</v>
       </c>
-      <c r="I306" s="75" t="s">
+      <c r="I306" s="78" t="s">
         <v>611</v>
       </c>
-      <c r="J306" s="76"/>
-      <c r="K306" s="75" t="n">
+      <c r="J306" s="79"/>
+      <c r="K306" s="78" t="n">
         <v>25</v>
       </c>
-      <c r="L306" s="77" t="s">
+      <c r="L306" s="80" t="s">
         <v>612</v>
       </c>
-      <c r="M306" s="76"/>
-      <c r="N306" s="75" t="n">
+      <c r="M306" s="79"/>
+      <c r="N306" s="78" t="n">
         <v>11</v>
       </c>
-      <c r="O306" s="76" t="s">
+      <c r="O306" s="79" t="s">
         <v>571</v>
       </c>
-      <c r="P306" s="75" t="n">
+      <c r="P306" s="78" t="n">
         <v>11</v>
       </c>
-      <c r="Q306" s="76"/>
-      <c r="R306" s="76" t="s">
-        <v>102</v>
-      </c>
-      <c r="S306" s="76" t="s">
-        <v>103</v>
-      </c>
-      <c r="T306" s="76"/>
-      <c r="U306" s="75" t="n">
+      <c r="Q306" s="79"/>
+      <c r="R306" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="S306" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="T306" s="79"/>
+      <c r="U306" s="78" t="n">
         <v>11</v>
       </c>
-      <c r="V306" s="76" t="s">
+      <c r="V306" s="79" t="s">
         <v>572</v>
       </c>
       <c r="W306" s="28"/>
@@ -21396,56 +21416,56 @@
       <c r="Y306" s="29"/>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A307" s="74"/>
-      <c r="B307" s="78" t="s">
+      <c r="A307" s="77"/>
+      <c r="B307" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="C307" s="78" t="s">
+      <c r="C307" s="81" t="s">
         <v>434</v>
       </c>
-      <c r="D307" s="79"/>
-      <c r="E307" s="78" t="n">
-        <v>20</v>
-      </c>
-      <c r="F307" s="80" t="s">
+      <c r="D307" s="82"/>
+      <c r="E307" s="81" t="n">
+        <v>20</v>
+      </c>
+      <c r="F307" s="83" t="s">
         <v>613</v>
       </c>
-      <c r="G307" s="79"/>
-      <c r="H307" s="78" t="s">
+      <c r="G307" s="82"/>
+      <c r="H307" s="81" t="s">
         <v>614</v>
       </c>
-      <c r="I307" s="78" t="s">
+      <c r="I307" s="81" t="s">
         <v>615</v>
       </c>
-      <c r="J307" s="79"/>
-      <c r="K307" s="78" t="n">
+      <c r="J307" s="82"/>
+      <c r="K307" s="81" t="n">
         <v>25</v>
       </c>
-      <c r="L307" s="80" t="s">
+      <c r="L307" s="83" t="s">
         <v>616</v>
       </c>
-      <c r="M307" s="79"/>
-      <c r="N307" s="78" t="n">
+      <c r="M307" s="82"/>
+      <c r="N307" s="81" t="n">
         <v>12</v>
       </c>
-      <c r="O307" s="79" t="s">
+      <c r="O307" s="82" t="s">
         <v>571</v>
       </c>
-      <c r="P307" s="78" t="n">
+      <c r="P307" s="81" t="n">
         <v>12</v>
       </c>
-      <c r="Q307" s="79"/>
-      <c r="R307" s="79" t="s">
-        <v>102</v>
-      </c>
-      <c r="S307" s="79" t="s">
-        <v>103</v>
-      </c>
-      <c r="T307" s="79"/>
-      <c r="U307" s="78" t="n">
+      <c r="Q307" s="82"/>
+      <c r="R307" s="82" t="s">
+        <v>102</v>
+      </c>
+      <c r="S307" s="82" t="s">
+        <v>103</v>
+      </c>
+      <c r="T307" s="82"/>
+      <c r="U307" s="81" t="n">
         <v>12</v>
       </c>
-      <c r="V307" s="79" t="s">
+      <c r="V307" s="82" t="s">
         <v>572</v>
       </c>
       <c r="W307" s="28"/>
@@ -21453,58 +21473,58 @@
       <c r="Y307" s="29"/>
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A308" s="74" t="s">
+      <c r="A308" s="77" t="s">
         <v>177</v>
       </c>
-      <c r="B308" s="75" t="s">
+      <c r="B308" s="78" t="s">
         <v>97</v>
       </c>
-      <c r="C308" s="75" t="s">
+      <c r="C308" s="78" t="s">
         <v>434</v>
       </c>
-      <c r="D308" s="76"/>
-      <c r="E308" s="75" t="n">
-        <v>20</v>
-      </c>
-      <c r="F308" s="77" t="s">
+      <c r="D308" s="79"/>
+      <c r="E308" s="78" t="n">
+        <v>20</v>
+      </c>
+      <c r="F308" s="80" t="s">
         <v>617</v>
       </c>
-      <c r="G308" s="76"/>
-      <c r="H308" s="75" t="s">
+      <c r="G308" s="79"/>
+      <c r="H308" s="78" t="s">
         <v>618</v>
       </c>
-      <c r="I308" s="75" t="s">
+      <c r="I308" s="78" t="s">
         <v>619</v>
       </c>
-      <c r="J308" s="76"/>
-      <c r="K308" s="75" t="n">
+      <c r="J308" s="79"/>
+      <c r="K308" s="78" t="n">
         <v>25</v>
       </c>
-      <c r="L308" s="77" t="s">
+      <c r="L308" s="80" t="s">
         <v>620</v>
       </c>
-      <c r="M308" s="76"/>
-      <c r="N308" s="75" t="n">
+      <c r="M308" s="79"/>
+      <c r="N308" s="78" t="n">
         <v>13</v>
       </c>
-      <c r="O308" s="76" t="s">
+      <c r="O308" s="79" t="s">
         <v>571</v>
       </c>
-      <c r="P308" s="75" t="n">
+      <c r="P308" s="78" t="n">
         <v>13</v>
       </c>
-      <c r="Q308" s="76"/>
-      <c r="R308" s="76" t="s">
-        <v>102</v>
-      </c>
-      <c r="S308" s="76" t="s">
-        <v>103</v>
-      </c>
-      <c r="T308" s="76"/>
-      <c r="U308" s="75" t="n">
+      <c r="Q308" s="79"/>
+      <c r="R308" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="S308" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="T308" s="79"/>
+      <c r="U308" s="78" t="n">
         <v>13</v>
       </c>
-      <c r="V308" s="76" t="s">
+      <c r="V308" s="79" t="s">
         <v>572</v>
       </c>
       <c r="W308" s="28"/>
@@ -21512,56 +21532,56 @@
       <c r="Y308" s="29"/>
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A309" s="74"/>
-      <c r="B309" s="78" t="s">
+      <c r="A309" s="77"/>
+      <c r="B309" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="C309" s="78" t="s">
+      <c r="C309" s="81" t="s">
         <v>434</v>
       </c>
-      <c r="D309" s="79"/>
-      <c r="E309" s="78" t="n">
-        <v>20</v>
-      </c>
-      <c r="F309" s="80" t="s">
+      <c r="D309" s="82"/>
+      <c r="E309" s="81" t="n">
+        <v>20</v>
+      </c>
+      <c r="F309" s="83" t="s">
         <v>621</v>
       </c>
-      <c r="G309" s="79"/>
-      <c r="H309" s="78" t="s">
+      <c r="G309" s="82"/>
+      <c r="H309" s="81" t="s">
         <v>622</v>
       </c>
-      <c r="I309" s="78" t="s">
+      <c r="I309" s="81" t="s">
         <v>623</v>
       </c>
-      <c r="J309" s="79"/>
-      <c r="K309" s="78" t="n">
+      <c r="J309" s="82"/>
+      <c r="K309" s="81" t="n">
         <v>25</v>
       </c>
-      <c r="L309" s="80" t="s">
+      <c r="L309" s="83" t="s">
         <v>624</v>
       </c>
-      <c r="M309" s="79"/>
-      <c r="N309" s="78" t="n">
+      <c r="M309" s="82"/>
+      <c r="N309" s="81" t="n">
         <v>14</v>
       </c>
-      <c r="O309" s="79" t="s">
+      <c r="O309" s="82" t="s">
         <v>571</v>
       </c>
-      <c r="P309" s="78" t="n">
+      <c r="P309" s="81" t="n">
         <v>14</v>
       </c>
-      <c r="Q309" s="79"/>
-      <c r="R309" s="79" t="s">
-        <v>102</v>
-      </c>
-      <c r="S309" s="79" t="s">
-        <v>103</v>
-      </c>
-      <c r="T309" s="79"/>
-      <c r="U309" s="78" t="n">
+      <c r="Q309" s="82"/>
+      <c r="R309" s="82" t="s">
+        <v>102</v>
+      </c>
+      <c r="S309" s="82" t="s">
+        <v>103</v>
+      </c>
+      <c r="T309" s="82"/>
+      <c r="U309" s="81" t="n">
         <v>14</v>
       </c>
-      <c r="V309" s="79" t="s">
+      <c r="V309" s="82" t="s">
         <v>572</v>
       </c>
       <c r="W309" s="28"/>
@@ -21569,58 +21589,58 @@
       <c r="Y309" s="29"/>
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A310" s="74" t="s">
+      <c r="A310" s="77" t="s">
         <v>180</v>
       </c>
-      <c r="B310" s="75" t="s">
+      <c r="B310" s="78" t="s">
         <v>97</v>
       </c>
-      <c r="C310" s="75" t="s">
+      <c r="C310" s="78" t="s">
         <v>434</v>
       </c>
-      <c r="D310" s="76"/>
-      <c r="E310" s="75" t="n">
-        <v>20</v>
-      </c>
-      <c r="F310" s="77" t="s">
+      <c r="D310" s="79"/>
+      <c r="E310" s="78" t="n">
+        <v>20</v>
+      </c>
+      <c r="F310" s="80" t="s">
         <v>625</v>
       </c>
-      <c r="G310" s="76"/>
-      <c r="H310" s="75" t="s">
+      <c r="G310" s="79"/>
+      <c r="H310" s="78" t="s">
         <v>626</v>
       </c>
-      <c r="I310" s="75" t="s">
+      <c r="I310" s="78" t="s">
         <v>627</v>
       </c>
-      <c r="J310" s="76"/>
-      <c r="K310" s="75" t="n">
+      <c r="J310" s="79"/>
+      <c r="K310" s="78" t="n">
         <v>25</v>
       </c>
-      <c r="L310" s="77" t="s">
+      <c r="L310" s="80" t="s">
         <v>628</v>
       </c>
-      <c r="M310" s="76"/>
-      <c r="N310" s="75" t="n">
+      <c r="M310" s="79"/>
+      <c r="N310" s="78" t="n">
         <v>15</v>
       </c>
-      <c r="O310" s="76" t="s">
+      <c r="O310" s="79" t="s">
         <v>571</v>
       </c>
-      <c r="P310" s="75" t="n">
+      <c r="P310" s="78" t="n">
         <v>15</v>
       </c>
-      <c r="Q310" s="76"/>
-      <c r="R310" s="76" t="s">
-        <v>102</v>
-      </c>
-      <c r="S310" s="76" t="s">
-        <v>103</v>
-      </c>
-      <c r="T310" s="76"/>
-      <c r="U310" s="75" t="n">
+      <c r="Q310" s="79"/>
+      <c r="R310" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="S310" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="T310" s="79"/>
+      <c r="U310" s="78" t="n">
         <v>15</v>
       </c>
-      <c r="V310" s="76" t="s">
+      <c r="V310" s="79" t="s">
         <v>572</v>
       </c>
       <c r="W310" s="28"/>
@@ -21628,56 +21648,56 @@
       <c r="Y310" s="29"/>
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A311" s="74"/>
-      <c r="B311" s="78" t="s">
+      <c r="A311" s="77"/>
+      <c r="B311" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="C311" s="78" t="s">
+      <c r="C311" s="81" t="s">
         <v>434</v>
       </c>
-      <c r="D311" s="79"/>
-      <c r="E311" s="78" t="n">
-        <v>20</v>
-      </c>
-      <c r="F311" s="80" t="s">
+      <c r="D311" s="82"/>
+      <c r="E311" s="81" t="n">
+        <v>20</v>
+      </c>
+      <c r="F311" s="83" t="s">
         <v>629</v>
       </c>
-      <c r="G311" s="79"/>
-      <c r="H311" s="78" t="s">
+      <c r="G311" s="82"/>
+      <c r="H311" s="81" t="s">
         <v>630</v>
       </c>
-      <c r="I311" s="78" t="s">
+      <c r="I311" s="81" t="s">
         <v>631</v>
       </c>
-      <c r="J311" s="79"/>
-      <c r="K311" s="78" t="n">
+      <c r="J311" s="82"/>
+      <c r="K311" s="81" t="n">
         <v>25</v>
       </c>
-      <c r="L311" s="80" t="s">
+      <c r="L311" s="83" t="s">
         <v>632</v>
       </c>
-      <c r="M311" s="79"/>
-      <c r="N311" s="78" t="n">
+      <c r="M311" s="82"/>
+      <c r="N311" s="81" t="n">
         <v>16</v>
       </c>
-      <c r="O311" s="79" t="s">
+      <c r="O311" s="82" t="s">
         <v>571</v>
       </c>
-      <c r="P311" s="78" t="n">
+      <c r="P311" s="81" t="n">
         <v>16</v>
       </c>
-      <c r="Q311" s="79"/>
-      <c r="R311" s="79" t="s">
-        <v>102</v>
-      </c>
-      <c r="S311" s="79" t="s">
-        <v>103</v>
-      </c>
-      <c r="T311" s="79"/>
-      <c r="U311" s="78" t="n">
+      <c r="Q311" s="82"/>
+      <c r="R311" s="82" t="s">
+        <v>102</v>
+      </c>
+      <c r="S311" s="82" t="s">
+        <v>103</v>
+      </c>
+      <c r="T311" s="82"/>
+      <c r="U311" s="81" t="n">
         <v>16</v>
       </c>
-      <c r="V311" s="79" t="s">
+      <c r="V311" s="82" t="s">
         <v>572</v>
       </c>
       <c r="W311" s="28"/>
@@ -23565,58 +23585,58 @@
       <c r="Y343" s="29"/>
     </row>
     <row r="344" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A344" s="74" t="s">
+      <c r="A344" s="77" t="s">
         <v>235</v>
       </c>
-      <c r="B344" s="75" t="s">
+      <c r="B344" s="78" t="s">
         <v>97</v>
       </c>
-      <c r="C344" s="75" t="s">
+      <c r="C344" s="78" t="s">
         <v>434</v>
       </c>
-      <c r="D344" s="76"/>
-      <c r="E344" s="75" t="n">
-        <v>20</v>
-      </c>
-      <c r="F344" s="77" t="s">
+      <c r="D344" s="79"/>
+      <c r="E344" s="78" t="n">
+        <v>20</v>
+      </c>
+      <c r="F344" s="80" t="s">
         <v>765</v>
       </c>
-      <c r="G344" s="76"/>
-      <c r="H344" s="75" t="s">
+      <c r="G344" s="79"/>
+      <c r="H344" s="78" t="s">
         <v>766</v>
       </c>
-      <c r="I344" s="75" t="s">
+      <c r="I344" s="78" t="s">
         <v>767</v>
       </c>
-      <c r="J344" s="76"/>
-      <c r="K344" s="75" t="n">
+      <c r="J344" s="79"/>
+      <c r="K344" s="78" t="n">
         <v>25</v>
       </c>
-      <c r="L344" s="77" t="s">
+      <c r="L344" s="80" t="s">
         <v>768</v>
       </c>
-      <c r="M344" s="76"/>
-      <c r="N344" s="75" t="n">
+      <c r="M344" s="79"/>
+      <c r="N344" s="78" t="n">
         <v>13</v>
       </c>
-      <c r="O344" s="76" t="s">
+      <c r="O344" s="79" t="s">
         <v>237</v>
       </c>
-      <c r="P344" s="75" t="n">
+      <c r="P344" s="78" t="n">
         <v>13</v>
       </c>
-      <c r="Q344" s="76"/>
-      <c r="R344" s="76" t="s">
-        <v>102</v>
-      </c>
-      <c r="S344" s="76" t="s">
-        <v>103</v>
-      </c>
-      <c r="T344" s="76"/>
-      <c r="U344" s="75" t="n">
+      <c r="Q344" s="79"/>
+      <c r="R344" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="S344" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="T344" s="79"/>
+      <c r="U344" s="78" t="n">
         <v>13</v>
       </c>
-      <c r="V344" s="76" t="s">
+      <c r="V344" s="79" t="s">
         <v>238</v>
       </c>
       <c r="W344" s="28" t="s">
@@ -23630,56 +23650,56 @@
       </c>
     </row>
     <row r="345" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A345" s="74"/>
-      <c r="B345" s="78" t="s">
+      <c r="A345" s="77"/>
+      <c r="B345" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="C345" s="78" t="s">
+      <c r="C345" s="81" t="s">
         <v>434</v>
       </c>
-      <c r="D345" s="79"/>
-      <c r="E345" s="78" t="n">
-        <v>20</v>
-      </c>
-      <c r="F345" s="80" t="s">
+      <c r="D345" s="82"/>
+      <c r="E345" s="81" t="n">
+        <v>20</v>
+      </c>
+      <c r="F345" s="83" t="s">
         <v>769</v>
       </c>
-      <c r="G345" s="79"/>
-      <c r="H345" s="78" t="s">
+      <c r="G345" s="82"/>
+      <c r="H345" s="81" t="s">
         <v>770</v>
       </c>
-      <c r="I345" s="78" t="s">
+      <c r="I345" s="81" t="s">
         <v>771</v>
       </c>
-      <c r="J345" s="79"/>
-      <c r="K345" s="78" t="n">
+      <c r="J345" s="82"/>
+      <c r="K345" s="81" t="n">
         <v>25</v>
       </c>
-      <c r="L345" s="80" t="s">
+      <c r="L345" s="83" t="s">
         <v>772</v>
       </c>
-      <c r="M345" s="79"/>
-      <c r="N345" s="78" t="n">
+      <c r="M345" s="82"/>
+      <c r="N345" s="81" t="n">
         <v>14</v>
       </c>
-      <c r="O345" s="79" t="s">
+      <c r="O345" s="82" t="s">
         <v>237</v>
       </c>
-      <c r="P345" s="78" t="n">
+      <c r="P345" s="81" t="n">
         <v>14</v>
       </c>
-      <c r="Q345" s="79"/>
-      <c r="R345" s="79" t="s">
-        <v>102</v>
-      </c>
-      <c r="S345" s="79" t="s">
-        <v>103</v>
-      </c>
-      <c r="T345" s="79"/>
-      <c r="U345" s="78" t="n">
+      <c r="Q345" s="82"/>
+      <c r="R345" s="82" t="s">
+        <v>102</v>
+      </c>
+      <c r="S345" s="82" t="s">
+        <v>103</v>
+      </c>
+      <c r="T345" s="82"/>
+      <c r="U345" s="81" t="n">
         <v>14</v>
       </c>
-      <c r="V345" s="79" t="s">
+      <c r="V345" s="82" t="s">
         <v>238</v>
       </c>
       <c r="W345" s="28"/>
@@ -23687,58 +23707,58 @@
       <c r="Y345" s="29"/>
     </row>
     <row r="346" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A346" s="74" t="s">
+      <c r="A346" s="77" t="s">
         <v>240</v>
       </c>
-      <c r="B346" s="75" t="s">
+      <c r="B346" s="78" t="s">
         <v>97</v>
       </c>
-      <c r="C346" s="75" t="s">
+      <c r="C346" s="78" t="s">
         <v>434</v>
       </c>
-      <c r="D346" s="76"/>
-      <c r="E346" s="75" t="n">
-        <v>20</v>
-      </c>
-      <c r="F346" s="77" t="s">
+      <c r="D346" s="79"/>
+      <c r="E346" s="78" t="n">
+        <v>20</v>
+      </c>
+      <c r="F346" s="80" t="s">
         <v>773</v>
       </c>
-      <c r="G346" s="76"/>
-      <c r="H346" s="75" t="s">
+      <c r="G346" s="79"/>
+      <c r="H346" s="78" t="s">
         <v>774</v>
       </c>
-      <c r="I346" s="75" t="s">
+      <c r="I346" s="78" t="s">
         <v>775</v>
       </c>
-      <c r="J346" s="76"/>
-      <c r="K346" s="75" t="n">
+      <c r="J346" s="79"/>
+      <c r="K346" s="78" t="n">
         <v>25</v>
       </c>
-      <c r="L346" s="77" t="s">
+      <c r="L346" s="80" t="s">
         <v>776</v>
       </c>
-      <c r="M346" s="76"/>
-      <c r="N346" s="75" t="n">
+      <c r="M346" s="79"/>
+      <c r="N346" s="78" t="n">
         <v>15</v>
       </c>
-      <c r="O346" s="76" t="s">
+      <c r="O346" s="79" t="s">
         <v>237</v>
       </c>
-      <c r="P346" s="75" t="n">
+      <c r="P346" s="78" t="n">
         <v>15</v>
       </c>
-      <c r="Q346" s="76"/>
-      <c r="R346" s="76" t="s">
-        <v>102</v>
-      </c>
-      <c r="S346" s="76" t="s">
-        <v>103</v>
-      </c>
-      <c r="T346" s="76"/>
-      <c r="U346" s="75" t="n">
+      <c r="Q346" s="79"/>
+      <c r="R346" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="S346" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="T346" s="79"/>
+      <c r="U346" s="78" t="n">
         <v>15</v>
       </c>
-      <c r="V346" s="76" t="s">
+      <c r="V346" s="79" t="s">
         <v>238</v>
       </c>
       <c r="W346" s="28"/>
@@ -23746,56 +23766,56 @@
       <c r="Y346" s="29"/>
     </row>
     <row r="347" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A347" s="74"/>
-      <c r="B347" s="78" t="s">
+      <c r="A347" s="77"/>
+      <c r="B347" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="C347" s="78" t="s">
+      <c r="C347" s="81" t="s">
         <v>434</v>
       </c>
-      <c r="D347" s="79"/>
-      <c r="E347" s="78" t="n">
-        <v>20</v>
-      </c>
-      <c r="F347" s="80" t="s">
+      <c r="D347" s="82"/>
+      <c r="E347" s="81" t="n">
+        <v>20</v>
+      </c>
+      <c r="F347" s="83" t="s">
         <v>777</v>
       </c>
-      <c r="G347" s="79"/>
-      <c r="H347" s="78" t="s">
+      <c r="G347" s="82"/>
+      <c r="H347" s="81" t="s">
         <v>778</v>
       </c>
-      <c r="I347" s="78" t="s">
+      <c r="I347" s="81" t="s">
         <v>779</v>
       </c>
-      <c r="J347" s="79"/>
-      <c r="K347" s="78" t="n">
+      <c r="J347" s="82"/>
+      <c r="K347" s="81" t="n">
         <v>25</v>
       </c>
-      <c r="L347" s="80" t="s">
+      <c r="L347" s="83" t="s">
         <v>780</v>
       </c>
-      <c r="M347" s="79"/>
-      <c r="N347" s="78" t="n">
+      <c r="M347" s="82"/>
+      <c r="N347" s="81" t="n">
         <v>16</v>
       </c>
-      <c r="O347" s="79" t="s">
+      <c r="O347" s="82" t="s">
         <v>237</v>
       </c>
-      <c r="P347" s="78" t="n">
+      <c r="P347" s="81" t="n">
         <v>16</v>
       </c>
-      <c r="Q347" s="79"/>
-      <c r="R347" s="79" t="s">
-        <v>102</v>
-      </c>
-      <c r="S347" s="79" t="s">
-        <v>103</v>
-      </c>
-      <c r="T347" s="79"/>
-      <c r="U347" s="78" t="n">
+      <c r="Q347" s="82"/>
+      <c r="R347" s="82" t="s">
+        <v>102</v>
+      </c>
+      <c r="S347" s="82" t="s">
+        <v>103</v>
+      </c>
+      <c r="T347" s="82"/>
+      <c r="U347" s="81" t="n">
         <v>16</v>
       </c>
-      <c r="V347" s="79" t="s">
+      <c r="V347" s="82" t="s">
         <v>238</v>
       </c>
       <c r="W347" s="28"/>

</xml_diff>